<commit_message>
Añadir test de github
</commit_message>
<xml_diff>
--- a/backend/myapp/scripts/microorganismos_detectados_con_ids.xlsx
+++ b/backend/myapp/scripts/microorganismos_detectados_con_ids.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beatr\Desktop\TFG INFORMATICA\Web Microbiota\backend\scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beatr\Desktop\TFG INFORMATICA\Web Microbiota\backend\myapp\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB94C483-D9C5-4685-9A19-DC4F8AF49718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DADCE4-70A7-4C7D-964A-0C61E3B8FDA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -8625,8 +8624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F807"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A553" workbookViewId="0">
+      <selection activeCell="B573" sqref="B573"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>